<commit_message>
100 days of coding challenge & tried to solve longest palindrome array problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonet\Desktop\Coding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B8FB26-91DC-40B4-A2AF-33D3F63EA26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4ED5748E-A24E-4A7F-9082-541AB6655121}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -36,9 +30,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>1. Arrays</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
     <t>3. Arrays</t>
   </si>
   <si>
-    <t>Remove duplicates from sorted array</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/remove-duplicates-from-sorted-array/</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>https://leetcode.com/problems/remove-element/</t>
   </si>
   <si>
-    <t>Remove duplicate</t>
-  </si>
-  <si>
     <t>5. Arrays</t>
   </si>
   <si>
@@ -138,22 +123,37 @@
     <t>https://leetcode.com/problems/product-of-array-except-self/</t>
   </si>
   <si>
-    <t>9. Arrays</t>
-  </si>
-  <si>
-    <t>Second Maximum Element</t>
-  </si>
-  <si>
-    <t>use the maximum element's index to find the second maximun element's index in an unordered array</t>
-  </si>
-  <si>
-    <t>Not a leetcode problem</t>
+    <t>Palindrome Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-number/</t>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>Short Notes</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>Remove Element</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -631,18 +631,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153FF699-133F-4181-9471-8E28AA2AB2FE}">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +675,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -689,140 +689,158 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>32</v>
-      </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="13" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="11" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
-        <v>40</v>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{88AFB6A4-C743-40BA-ABB7-FB888C68668A}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{2AADB28D-456B-4729-94EF-1DCAA0E356B2}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{E5A3B617-CAF7-4626-A347-850659EA75E3}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{6FD8CFE9-F732-42F3-B3B0-02AA70272057}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{2DDBD9FD-1A45-4362-839F-E99B76F37EA2}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{6A16F812-509E-4C84-8BD5-3C0CCE3B52AA}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{42BBD10C-4A68-4D62-86E7-C568452EAA67}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{C9C25E2A-C385-48DF-942C-0B0D46F74C69}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>

</xml_diff>

<commit_message>
Day-1 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -148,13 +148,31 @@
   </si>
   <si>
     <t>Remove Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindromic-substring/</t>
+  </si>
+  <si>
+    <t>Longest Palindrome Substring</t>
+  </si>
+  <si>
+    <t>15. Dynamic Programming</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/running-sum-of-1d-array/</t>
+  </si>
+  <si>
+    <t>Running Sum of 1d Array</t>
+  </si>
+  <si>
+    <t>16. Arrays</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +217,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +249,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -291,12 +321,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -323,10 +354,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -631,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -639,15 +672,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="107.140625" customWidth="1"/>
     <col min="4" max="4" width="65.7109375" customWidth="1"/>
@@ -829,6 +862,28 @@
       </c>
       <c r="D14" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved remove duplicates from sorted/unsorted list leetcode problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -162,10 +162,34 @@
     <t>https://leetcode.com/problems/running-sum-of-1d-array/</t>
   </si>
   <si>
-    <t>Running Sum of 1d Array</t>
-  </si>
-  <si>
     <t>16. Arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/transpose-matrix/</t>
+  </si>
+  <si>
+    <t>17.Arrays</t>
+  </si>
+  <si>
+    <t>Running Sum of 1d Array (June Day1)</t>
+  </si>
+  <si>
+    <t>Transpose Matrix (June Day2)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list/</t>
+  </si>
+  <si>
+    <t>18. Linked List</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List</t>
+  </si>
+  <si>
+    <t>14. Arrays</t>
+  </si>
+  <si>
+    <t>13. Linked List</t>
   </si>
 </sst>
 </file>
@@ -672,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +860,7 @@
       <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -844,23 +868,29 @@
       <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
       <c r="B13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
       <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -871,19 +901,41 @@
       <c r="B15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -896,8 +948,16 @@
     <hyperlink ref="D8" r:id="rId6"/>
     <hyperlink ref="D9" r:id="rId7"/>
     <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D18" r:id="rId9"/>
+    <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D13" r:id="rId14"/>
+    <hyperlink ref="D12" r:id="rId15"/>
+    <hyperlink ref="D11" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-3 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -190,13 +190,22 @@
   </si>
   <si>
     <t>13. Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/range-sum-query-2d-immutable/</t>
+  </si>
+  <si>
+    <t>Range Sum Query 2D - Immutable</t>
+  </si>
+  <si>
+    <t>19. Matrix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +257,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -269,13 +285,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -349,9 +365,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -375,10 +391,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -696,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +779,7 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
@@ -776,7 +793,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
@@ -790,7 +807,7 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -804,7 +821,7 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C7" t="s">
@@ -818,7 +835,7 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
@@ -832,7 +849,7 @@
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
@@ -846,7 +863,7 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
@@ -857,7 +874,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -865,7 +882,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -876,7 +893,7 @@
       <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -887,7 +904,7 @@
       <c r="A14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -898,7 +915,7 @@
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -909,7 +926,7 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -920,7 +937,7 @@
       <c r="A17" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="14" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -931,11 +948,22 @@
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -956,8 +984,9 @@
     <hyperlink ref="D13" r:id="rId14"/>
     <hyperlink ref="D12" r:id="rId15"/>
     <hyperlink ref="D11" r:id="rId16"/>
+    <hyperlink ref="D19" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-4 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -171,12 +171,6 @@
     <t>17.Arrays</t>
   </si>
   <si>
-    <t>Running Sum of 1d Array (June Day1)</t>
-  </si>
-  <si>
-    <t>Transpose Matrix (June Day2)</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list/</t>
   </si>
   <si>
@@ -195,10 +189,25 @@
     <t>https://leetcode.com/problems/range-sum-query-2d-immutable/</t>
   </si>
   <si>
-    <t>Range Sum Query 2D - Immutable</t>
-  </si>
-  <si>
     <t>19. Matrix</t>
+  </si>
+  <si>
+    <t>Running Sum of 1d Array (June Day-1)</t>
+  </si>
+  <si>
+    <t>Transpose Matrix (June Day-2)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/n-queens/</t>
+  </si>
+  <si>
+    <t>20. Backtracking</t>
+  </si>
+  <si>
+    <t>N-Queens (June Day-4)</t>
+  </si>
+  <si>
+    <t>Range Sum Query 2D - Immutable (June Day-3)</t>
   </si>
 </sst>
 </file>
@@ -265,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +382,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -396,6 +411,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -705,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,16 +729,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="3" max="3" width="107.140625" customWidth="1"/>
     <col min="4" max="4" width="65.7109375" customWidth="1"/>
   </cols>
@@ -891,7 +907,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>38</v>
@@ -902,7 +918,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>16</v>
@@ -927,7 +943,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>46</v>
@@ -938,7 +954,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>48</v>
@@ -946,24 +962,35 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -985,8 +1012,9 @@
     <hyperlink ref="D12" r:id="rId15"/>
     <hyperlink ref="D11" r:id="rId16"/>
     <hyperlink ref="D19" r:id="rId17"/>
+    <hyperlink ref="D20" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-5 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -208,6 +208,36 @@
   </si>
   <si>
     <t>Range Sum Query 2D - Immutable (June Day-3)</t>
+  </si>
+  <si>
+    <t>N-Queens II (June Day-5)</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/n-queens-ii/</t>
+  </si>
+  <si>
+    <t>21. Backtracking</t>
+  </si>
+  <si>
+    <t>22. Dynamic Programming</t>
+  </si>
+  <si>
+    <t>It's basically a fibonacci series if you break the logic</t>
+  </si>
+  <si>
+    <t>9. Numbers</t>
+  </si>
+  <si>
+    <t>10. Numbers</t>
+  </si>
+  <si>
+    <t>map all the given values with given characters. If the current value is lesser than next value, the subtract it. For vice versa, add them up.</t>
   </si>
 </sst>
 </file>
@@ -254,13 +284,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF212121"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -273,8 +296,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,14 +329,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -376,13 +399,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -404,16 +428,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -721,7 +744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,13 +804,13 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -795,13 +818,13 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -809,13 +832,13 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -823,13 +846,13 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -837,13 +860,13 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -851,13 +874,13 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -865,13 +888,13 @@
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -879,29 +902,38 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -909,10 +941,10 @@
       <c r="A13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -920,10 +952,10 @@
       <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -931,10 +963,10 @@
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -942,10 +974,10 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -953,10 +985,10 @@
       <c r="A17" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -964,10 +996,10 @@
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -975,10 +1007,10 @@
       <c r="A19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -986,11 +1018,36 @@
       <c r="A20" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1013,8 +1070,10 @@
     <hyperlink ref="D11" r:id="rId16"/>
     <hyperlink ref="D19" r:id="rId17"/>
     <hyperlink ref="D20" r:id="rId18"/>
+    <hyperlink ref="D22" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-6 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>map all the given values with given characters. If the current value is lesser than next value, the subtract it. For vice versa, add them up.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/intersection-of-two-linked-lists/</t>
+  </si>
+  <si>
+    <t>23. Linked List</t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists (June Day-6)</t>
   </si>
 </sst>
 </file>
@@ -744,7 +753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,6 +1057,17 @@
       </c>
       <c r="D22" s="9" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1072,8 +1092,9 @@
     <hyperlink ref="D20" r:id="rId18"/>
     <hyperlink ref="D22" r:id="rId19"/>
     <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D23" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved 2 questions from leetcode
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>Intersection of Two Linked Lists (June Day-6)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-average-subarray-i/</t>
+  </si>
+  <si>
+    <t>Maximum Average Subarray I</t>
+  </si>
+  <si>
+    <t>24. Sliding Window</t>
   </si>
 </sst>
 </file>
@@ -753,7 +762,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -761,7 +770,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
@@ -1068,6 +1077,17 @@
       </c>
       <c r="D23" s="9" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1093,8 +1113,9 @@
     <hyperlink ref="D22" r:id="rId19"/>
     <hyperlink ref="D21" r:id="rId20"/>
     <hyperlink ref="D23" r:id="rId21"/>
+    <hyperlink ref="D24" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-8 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Longest Palindrome Substring</t>
   </si>
   <si>
-    <t>15. Dynamic Programming</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/running-sum-of-1d-array/</t>
   </si>
   <si>
@@ -225,18 +222,9 @@
     <t>21. Backtracking</t>
   </si>
   <si>
-    <t>22. Dynamic Programming</t>
-  </si>
-  <si>
-    <t>It's basically a fibonacci series if you break the logic</t>
-  </si>
-  <si>
     <t>9. Numbers</t>
   </si>
   <si>
-    <t>10. Numbers</t>
-  </si>
-  <si>
     <t>map all the given values with given characters. If the current value is lesser than next value, the subtract it. For vice versa, add them up.</t>
   </si>
   <si>
@@ -256,6 +244,54 @@
   </si>
   <si>
     <t>24. Sliding Window</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/fibonacci-number/</t>
+  </si>
+  <si>
+    <t>Fibonacci Number</t>
+  </si>
+  <si>
+    <t>26. DP</t>
+  </si>
+  <si>
+    <t>25. DP</t>
+  </si>
+  <si>
+    <t>22. DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>27. Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>28. String</t>
+  </si>
+  <si>
+    <t>15. DP + String</t>
+  </si>
+  <si>
+    <t>10. String</t>
+  </si>
+  <si>
+    <t>It's basically a fibonacci series if you break the logic.</t>
   </si>
 </sst>
 </file>
@@ -424,7 +460,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -452,6 +488,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -762,7 +799,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -770,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +969,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>34</v>
@@ -943,13 +980,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>37</v>
@@ -957,7 +994,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>38</v>
@@ -968,7 +1005,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>16</v>
@@ -979,7 +1016,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>44</v>
@@ -990,104 +1027,148 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="D26" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>76</v>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1114,8 +1195,12 @@
     <hyperlink ref="D21" r:id="rId20"/>
     <hyperlink ref="D23" r:id="rId21"/>
     <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D25" r:id="rId23"/>
+    <hyperlink ref="D26" r:id="rId24"/>
+    <hyperlink ref="D27" r:id="rId25"/>
+    <hyperlink ref="D28" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-9 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>It's basically a fibonacci series if you break the logic.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t>29. Arrays</t>
+  </si>
+  <si>
+    <t>As array is sorted so we can use two pointers. First pointer will point to first index &amp; 2nd pointer will point to last index. O(n)</t>
   </si>
 </sst>
 </file>
@@ -358,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -488,7 +506,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -799,7 +817,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -807,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1149,7 @@
       <c r="A25" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -1169,6 +1187,20 @@
       </c>
       <c r="D28" s="9" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1199,8 +1231,9 @@
     <hyperlink ref="D26" r:id="rId24"/>
     <hyperlink ref="D27" r:id="rId25"/>
     <hyperlink ref="D28" r:id="rId26"/>
+    <hyperlink ref="D29" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-10 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -87,9 +87,6 @@
     <t>If val is matches with the element in the array, put the element in temp index location &amp; increament the temp value</t>
   </si>
   <si>
-    <t>Merge Sorted Array</t>
-  </si>
-  <si>
     <t>6. Arrays</t>
   </si>
   <si>
@@ -297,13 +294,52 @@
     <t>https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/</t>
   </si>
   <si>
-    <t>Two Sum II - Input Array Is Sorted</t>
-  </si>
-  <si>
     <t>29. Arrays</t>
   </si>
   <si>
     <t>As array is sorted so we can use two pointers. First pointer will point to first index &amp; 2nd pointer will point to last index. O(n)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-all-anagrams-in-a-string/</t>
+  </si>
+  <si>
+    <t>30. String</t>
+  </si>
+  <si>
+    <t>Find All Anagrams in a String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-palindromic-subsequences/</t>
+  </si>
+  <si>
+    <t>31. String</t>
+  </si>
+  <si>
+    <t>Remove Palindromic Subsequences (June Day-8)</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array Is Sorted (June Day-9)</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array (June Day-7)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/</t>
+  </si>
+  <si>
+    <t>32. Sliding Window + String</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters (June Day-10)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-two-numbers/</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>33. Linked List</t>
   </si>
 </sst>
 </file>
@@ -370,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +437,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,12 +549,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -817,7 +865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -825,18 +873,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="3" width="107.140625" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="150.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
@@ -861,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>5</v>
@@ -877,7 +925,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -891,7 +939,7 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
@@ -905,8 +953,8 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>41</v>
+      <c r="B5" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -919,7 +967,7 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -933,8 +981,8 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>42</v>
+      <c r="B7" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -945,87 +993,87 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -1034,173 +1082,217 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>44</v>
+        <v>87</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="D18" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="D23" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="11" t="s">
         <v>73</v>
       </c>
+      <c r="B24" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="D24" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="11" t="s">
         <v>78</v>
       </c>
+      <c r="B26" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="D26" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="11" t="s">
         <v>83</v>
       </c>
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="D27" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="11" t="s">
         <v>86</v>
       </c>
+      <c r="B28" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="D28" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>91</v>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1232,8 +1324,12 @@
     <hyperlink ref="D27" r:id="rId25"/>
     <hyperlink ref="D28" r:id="rId26"/>
     <hyperlink ref="D29" r:id="rId27"/>
+    <hyperlink ref="D30" r:id="rId28"/>
+    <hyperlink ref="D31" r:id="rId29"/>
+    <hyperlink ref="D32" r:id="rId30"/>
+    <hyperlink ref="D33" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-11 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -340,6 +340,15 @@
   </si>
   <si>
     <t>33. Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-operations-to-reduce-x-to-zero/</t>
+  </si>
+  <si>
+    <t>34. Arrays</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Reduce X to Zero</t>
   </si>
 </sst>
 </file>
@@ -865,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -873,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1302,17 @@
       </c>
       <c r="D33" s="9" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1328,8 +1348,9 @@
     <hyperlink ref="D31" r:id="rId29"/>
     <hyperlink ref="D32" r:id="rId30"/>
     <hyperlink ref="D33" r:id="rId31"/>
+    <hyperlink ref="D34" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tried to solve some string questions
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -349,6 +349,15 @@
   </si>
   <si>
     <t>Minimum Operations to Reduce X to Zero</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-all-occurrences-of-a-substring/</t>
+  </si>
+  <si>
+    <t>Remove All Occurrences of a Substring</t>
+  </si>
+  <si>
+    <t>35. String</t>
   </si>
 </sst>
 </file>
@@ -874,7 +883,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -882,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,6 +1322,17 @@
       </c>
       <c r="D34" s="9" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1349,8 +1369,9 @@
     <hyperlink ref="D32" r:id="rId30"/>
     <hyperlink ref="D33" r:id="rId31"/>
     <hyperlink ref="D34" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-12 for June Challenge & deleting ss thinking that was useless
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -358,6 +358,15 @@
   </si>
   <si>
     <t>35. String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-erasure-value/submissions/</t>
+  </si>
+  <si>
+    <t>Maximum Erasure Value</t>
+  </si>
+  <si>
+    <t>36. Arrays</t>
   </si>
 </sst>
 </file>
@@ -891,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,6 +1342,17 @@
       </c>
       <c r="D35" s="9" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1370,8 +1390,9 @@
     <hyperlink ref="D33" r:id="rId31"/>
     <hyperlink ref="D34" r:id="rId32"/>
     <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="D36" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-13 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -360,13 +360,34 @@
     <t>35. String</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/maximum-erasure-value/submissions/</t>
-  </si>
-  <si>
     <t>Maximum Erasure Value</t>
   </si>
   <si>
     <t>36. Arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-an-array/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-erasure-value/</t>
+  </si>
+  <si>
+    <t>Sort an Array</t>
+  </si>
+  <si>
+    <t>37. Arrays</t>
+  </si>
+  <si>
+    <t>use merge sort technique which is faster than any other sorting methods. Time Complexity 0(nlongn) even in worst time.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/triangle/</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>38. DP</t>
   </si>
 </sst>
 </file>
@@ -900,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,13 +1367,38 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>113</v>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1391,8 +1437,10 @@
     <hyperlink ref="D34" r:id="rId32"/>
     <hyperlink ref="D35" r:id="rId33"/>
     <hyperlink ref="D36" r:id="rId34"/>
+    <hyperlink ref="D37" r:id="rId35"/>
+    <hyperlink ref="D38" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-14 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>38. DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/delete-operation-for-two-strings/</t>
+  </si>
+  <si>
+    <t>39. String + DP</t>
+  </si>
+  <si>
+    <t>Delete Operation for Two Strings</t>
+  </si>
+  <si>
+    <t>The minimum number of steps = length of word1 + length of word2 - (2 * length of LCS)</t>
   </si>
 </sst>
 </file>
@@ -913,7 +925,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -921,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,6 +1411,20 @@
       </c>
       <c r="D38" s="9" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1439,8 +1465,9 @@
     <hyperlink ref="D36" r:id="rId34"/>
     <hyperlink ref="D37" r:id="rId35"/>
     <hyperlink ref="D38" r:id="rId36"/>
+    <hyperlink ref="D39" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-15 for June Challenge
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -348,9 +348,6 @@
     <t>34. Arrays</t>
   </si>
   <si>
-    <t>Minimum Operations to Reduce X to Zero</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/remove-all-occurrences-of-a-substring/</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
     <t>35. String</t>
   </si>
   <si>
-    <t>Maximum Erasure Value</t>
-  </si>
-  <si>
     <t>36. Arrays</t>
   </si>
   <si>
@@ -384,9 +378,6 @@
     <t>https://leetcode.com/problems/triangle/</t>
   </si>
   <si>
-    <t>Triangle</t>
-  </si>
-  <si>
     <t>38. DP</t>
   </si>
   <si>
@@ -396,10 +387,40 @@
     <t>39. String + DP</t>
   </si>
   <si>
-    <t>Delete Operation for Two Strings</t>
-  </si>
-  <si>
     <t>The minimum number of steps = length of word1 + length of word2 - (2 * length of LCS) or just return m - c[m][n] + n - c[m][n]</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-increasing-subsequence/</t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-string-chain/</t>
+  </si>
+  <si>
+    <t>Same as LIS, just sort the list according to their size.</t>
+  </si>
+  <si>
+    <t>40. Array + DP</t>
+  </si>
+  <si>
+    <t>41. String + DP</t>
+  </si>
+  <si>
+    <t>Longest String Chain (June Day-15)</t>
+  </si>
+  <si>
+    <t>Delete Operation for Two Strings (June Day-14)</t>
+  </si>
+  <si>
+    <t>Triangle (June Day-13)</t>
+  </si>
+  <si>
+    <t>Maximum Erasure Value (June Day-12)</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Reduce X to Zero (June Day-11)</t>
   </si>
 </sst>
 </file>
@@ -925,7 +946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -933,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1381,7 @@
         <v>108</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>107</v>
@@ -1368,63 +1389,88 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
         <v>117</v>
       </c>
-      <c r="C37" t="s">
-        <v>119</v>
-      </c>
       <c r="D37" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="D40" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="C39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1466,8 +1512,10 @@
     <hyperlink ref="D37" r:id="rId35"/>
     <hyperlink ref="D38" r:id="rId36"/>
     <hyperlink ref="D39" r:id="rId37"/>
+    <hyperlink ref="D40" r:id="rId38"/>
+    <hyperlink ref="D41" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>